<commit_message>
formatted json file to add for Yahoo
</commit_message>
<xml_diff>
--- a/upload/UploadTemplate.xlsx
+++ b/upload/UploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alvinsoh/Documents/Heroku/asoh-flask-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F527CC41-12DF-5C4D-9B36-6D347A42BC7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D234E19-69AA-6E41-B4A7-636729EBDAC5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AppNexus" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Segment ID</t>
   </si>
@@ -197,6 +197,21 @@
   </si>
   <si>
     <t>Purchase Category - Reach - Healthy Food Buyers - Damn Poor People - Even Poorer People</t>
+  </si>
+  <si>
+    <t>Just random segment 4444</t>
+  </si>
+  <si>
+    <t>Just random segment 1111</t>
+  </si>
+  <si>
+    <t>Just random segment 2222</t>
+  </si>
+  <si>
+    <t>Just random segment 3333</t>
+  </si>
+  <si>
+    <t>taxoapitest</t>
   </si>
 </sst>
 </file>
@@ -1214,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1277,51 +1292,51 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>31804</v>
-      </c>
-      <c r="B3">
-        <v>4427</v>
+        <v>32048</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <v>3</v>
       </c>
-      <c r="G3" s="1">
-        <v>1.5</v>
+      <c r="G3">
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>32048</v>
+        <v>31804</v>
       </c>
       <c r="B4">
-        <v>32039</v>
+        <v>31804</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>3</v>
       </c>
-      <c r="G4">
-        <v>0</v>
+      <c r="G4" s="1">
+        <v>1.5</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1331,60 +1346,78 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27763304-9429-BE47-B12E-8F44F8D57B16}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4444</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1111</v>
       </c>
       <c r="B4" t="s">
         <v>33</v>
       </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2222</v>
       </c>
       <c r="B5" t="s">
         <v>34</v>
       </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3333</v>
       </c>
       <c r="B6" t="s">
         <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>